<commit_message>
fix series lable on j settings graph
</commit_message>
<xml_diff>
--- a/mac mini r5 eval.xlsx
+++ b/mac mini r5 eval.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="15195" windowHeight="9675" tabRatio="815" activeTab="5"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="15195" windowHeight="9675" tabRatio="815"/>
   </bookViews>
   <sheets>
     <sheet name="j settings" sheetId="20" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>Dual i7 2.7 GHz SSD</t>
   </si>
   <si>
-    <t>Dual i7 2.7 GHz 5400rpm</t>
-  </si>
-  <si>
     <t>Quad i7 2.0 GHz SSD -j2</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   <si>
     <t>I got 345 by adjusting until the number of machines needed for the existing hardware equaled the number of minis we have in production in that pool now</t>
   </si>
+  <si>
+    <t>Dual i5 2.7 GHz 5400rpm</t>
+  </si>
 </sst>
 </file>
 
@@ -258,7 +258,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -313,27 +313,21 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -381,6 +375,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -667,7 +667,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dual i7 2.7 GHz 5400rpm</c:v>
+                  <c:v>Dual i5 2.7 GHz 5400rpm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -726,7 +726,6 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="b"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -734,11 +733,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="195547648"/>
-        <c:axId val="195547072"/>
+        <c:axId val="118287168"/>
+        <c:axId val="118287744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="195547648"/>
+        <c:axId val="118287168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -769,13 +768,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195547072"/>
+        <c:crossAx val="118287744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="195547072"/>
+        <c:axId val="118287744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4750"/>
@@ -807,7 +806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195547648"/>
+        <c:crossAx val="118287168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="250"/>
@@ -860,7 +859,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1107,11 +1105,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1931264"/>
-        <c:axId val="144858432"/>
+        <c:axId val="41771008"/>
+        <c:axId val="118290048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1931264"/>
+        <c:axId val="41771008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1118,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144858432"/>
+        <c:crossAx val="118290048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1128,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144858432"/>
+        <c:axId val="118290048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1139,7 +1137,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1931264"/>
+        <c:crossAx val="41771008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1197,7 +1195,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1396,11 +1393,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="62041600"/>
-        <c:axId val="154624576"/>
+        <c:axId val="41348608"/>
+        <c:axId val="41885696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62041600"/>
+        <c:axId val="41348608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,7 +1406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154624576"/>
+        <c:crossAx val="41885696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1417,7 +1414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154624576"/>
+        <c:axId val="41885696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,14 +1455,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62041600"/>
+        <c:crossAx val="41348608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1514,7 +1510,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1758,11 +1753,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="97261056"/>
-        <c:axId val="154631488"/>
+        <c:axId val="42014208"/>
+        <c:axId val="41888000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97261056"/>
+        <c:axId val="42014208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1771,7 +1766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154631488"/>
+        <c:crossAx val="41888000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1779,7 +1774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154631488"/>
+        <c:axId val="41888000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -1804,14 +1799,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97261056"/>
+        <c:crossAx val="42014208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -1820,7 +1814,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1866,7 +1859,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2220,11 +2212,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41060352"/>
-        <c:axId val="154046976"/>
+        <c:axId val="41965056"/>
+        <c:axId val="41890304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41060352"/>
+        <c:axId val="41965056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2233,7 +2225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154046976"/>
+        <c:crossAx val="41890304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2241,7 +2233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154046976"/>
+        <c:axId val="41890304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2279,14 +2271,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41060352"/>
+        <c:crossAx val="41965056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2331,7 +2322,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2344,9 +2334,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Dual i7 2.7GHz -j4</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -2465,11 +2452,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="121937920"/>
-        <c:axId val="122095296"/>
+        <c:axId val="42373120"/>
+        <c:axId val="41893184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121937920"/>
+        <c:axId val="42373120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2479,7 +2466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122095296"/>
+        <c:crossAx val="41893184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2487,7 +2474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122095296"/>
+        <c:axId val="41893184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2518,21 +2505,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121937920"/>
+        <c:crossAx val="42373120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2582,7 +2567,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2595,9 +2579,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Dual i7 2.7GHz -j4</c:v>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -2678,11 +2659,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="122606592"/>
-        <c:axId val="122097024"/>
+        <c:axId val="41773568"/>
+        <c:axId val="42853504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="122606592"/>
+        <c:axId val="41773568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2691,7 +2672,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122097024"/>
+        <c:crossAx val="42853504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2699,7 +2680,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122097024"/>
+        <c:axId val="42853504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2722,21 +2703,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122606592"/>
+        <c:crossAx val="41773568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2998,25 +2977,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:G3" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="A2:G3"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="clone" dataDxfId="1">
+    <tableColumn id="1" name="clone" dataDxfId="23">
       <calculatedColumnFormula>('dual-i7-hd-j8'!A3-'dual-i7-ssd-j8'!A3)/'dual-i7-hd-j8'!A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="build" dataDxfId="23">
+    <tableColumn id="2" name="build" dataDxfId="22">
       <calculatedColumnFormula>('dual-i7-hd-j4'!B4-'dual-i7-ssd-j4'!B4)/'dual-i7-hd-j4'!B4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="package" dataDxfId="22">
+    <tableColumn id="3" name="package" dataDxfId="21">
       <calculatedColumnFormula>('dual-i7-hd-j4'!C4-'dual-i7-ssd-j4'!C4)/'dual-i7-hd-j4'!C4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="packagetests" dataDxfId="21">
+    <tableColumn id="4" name="packagetests" dataDxfId="20">
       <calculatedColumnFormula>('dual-i7-hd-j4'!D4-'dual-i7-ssd-j4'!D4)/'dual-i7-hd-j4'!D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="symbols" dataDxfId="20">
+    <tableColumn id="5" name="symbols" dataDxfId="19">
       <calculatedColumnFormula>('dual-i7-hd-j4'!E4-'dual-i7-ssd-j4'!E4)/'dual-i7-hd-j4'!E4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="clobber" dataDxfId="19">
+    <tableColumn id="6" name="clobber" dataDxfId="18">
       <calculatedColumnFormula>('dual-i7-hd-j4'!F4-'dual-i7-ssd-j4'!F4)/'dual-i7-hd-j4'!F4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="total" dataDxfId="18">
+    <tableColumn id="7" name="total" dataDxfId="17">
       <calculatedColumnFormula>('dual-i7-hd-j4'!G4-'dual-i7-ssd-j4'!G4)/'dual-i7-hd-j4'!G4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3185,28 +3164,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table69" displayName="Table69" ref="A7:G8" totalsRowShown="0" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table69" displayName="Table69" ref="A7:G8" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A7:G8"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="clone" dataDxfId="0">
+    <tableColumn id="1" name="clone" dataDxfId="15">
       <calculatedColumnFormula>'dual-i7-hd-j4'!A4-'dual-i7-ssd-j4'!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="build" dataDxfId="16">
+    <tableColumn id="2" name="build" dataDxfId="14">
       <calculatedColumnFormula>'dual-i7-hd-j4'!B9-'dual-i7-ssd-j4'!B9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="package" dataDxfId="15">
+    <tableColumn id="3" name="package" dataDxfId="13">
       <calculatedColumnFormula>'dual-i7-hd-j4'!C9-'dual-i7-ssd-j4'!C9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="packagetests" dataDxfId="14">
+    <tableColumn id="4" name="packagetests" dataDxfId="12">
       <calculatedColumnFormula>'dual-i7-hd-j4'!D9-'dual-i7-ssd-j4'!D9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="symbols" dataDxfId="13">
+    <tableColumn id="5" name="symbols" dataDxfId="11">
       <calculatedColumnFormula>'dual-i7-hd-j4'!E9-'dual-i7-ssd-j4'!E9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="clobber" dataDxfId="12">
+    <tableColumn id="6" name="clobber" dataDxfId="10">
       <calculatedColumnFormula>'dual-i7-hd-j4'!F9-'dual-i7-ssd-j4'!F9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="total" dataDxfId="11">
+    <tableColumn id="7" name="total" dataDxfId="9">
       <calculatedColumnFormula>'dual-i7-hd-j4'!G9-'dual-i7-ssd-j4'!G9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3279,16 +3258,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="quadi7ssdj4" displayName="quadi7ssdj4" ref="A7:G175" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="quadi7ssdj4" displayName="quadi7ssdj4" ref="A7:G175" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A7:G175"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="clone" dataDxfId="8"/>
-    <tableColumn id="2" name="build" dataDxfId="7"/>
-    <tableColumn id="3" name="package" dataDxfId="6"/>
-    <tableColumn id="4" name="packagetests" dataDxfId="5"/>
-    <tableColumn id="5" name="symbols" dataDxfId="4"/>
-    <tableColumn id="6" name="clobber" dataDxfId="3"/>
-    <tableColumn id="7" name="total" dataDxfId="2"/>
+    <tableColumn id="1" name="clone" dataDxfId="6"/>
+    <tableColumn id="2" name="build" dataDxfId="5"/>
+    <tableColumn id="3" name="package" dataDxfId="4"/>
+    <tableColumn id="4" name="packagetests" dataDxfId="3"/>
+    <tableColumn id="5" name="symbols" dataDxfId="2"/>
+    <tableColumn id="6" name="clobber" dataDxfId="1"/>
+    <tableColumn id="7" name="total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3663,8 +3642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,10 +3667,10 @@
         <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3834,26 +3813,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -3886,15 +3865,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -4074,15 +4053,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -4309,26 +4288,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -4391,15 +4370,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -5109,26 +5088,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -5161,15 +5140,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -5418,26 +5397,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -5470,15 +5449,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -5773,15 +5752,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -5985,26 +5964,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -6067,15 +6046,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -9498,26 +9477,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -9550,15 +9529,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -10037,26 +10016,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -10089,15 +10068,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -10370,15 +10349,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -10562,107 +10541,107 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="11">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9">
         <f>('moz2-darwin10-data'!$A$22-'quad-i7-ssd-j12'!$B$3)/60</f>
         <v>113.06166666666667</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>1599</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="8">
         <f>C2/$B2</f>
         <v>14.142724471895868</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="8">
         <f>($C2 * 0.95)/$B2</f>
         <v>13.435588248301075</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <f>($C2 * 0.9)/$B2</f>
         <v>12.728452024706282</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="8">
         <f>($C2 * 0.75)/$B2</f>
         <v>10.607043353921901</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="11">
+        <v>47</v>
+      </c>
+      <c r="B3" s="9">
         <f>('moz2-darwin10-data'!$A$22-'dual-i7-ssd-j4'!$B$4)/60</f>
         <v>105.90203703703703</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>1699</v>
       </c>
-      <c r="D3" s="10">
-        <f t="shared" ref="D3:E3" si="0">C3/$B3</f>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3" si="0">C3/$B3</f>
         <v>16.043128607675509</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <f t="shared" ref="E3:E5" si="1">($C3 * 0.95)/$B3</f>
         <v>15.240972177291733</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <f t="shared" ref="F3:F5" si="2">($C3 * 0.9)/$B3</f>
         <v>14.438815746907958</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <f t="shared" ref="G3:G5" si="3">($C3 * 0.75)/$B3</f>
         <v>12.032346455756631</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="11">
+        <v>48</v>
+      </c>
+      <c r="B4" s="9">
         <f>('moz2-darwin10-data'!$A$22-'dual-i7-hd-j4'!$B$4) / 60</f>
         <v>103.80362068965518</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>1249</v>
       </c>
-      <c r="D4" s="10">
-        <f t="shared" ref="D4:E4" si="4">C4/$B4</f>
+      <c r="D4" s="8">
+        <f t="shared" ref="D4" si="4">C4/$B4</f>
         <v>12.032335593901614</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <f t="shared" si="1"/>
         <v>11.430718814206534</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <f t="shared" si="2"/>
         <v>10.829102034511454</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="8">
         <f t="shared" si="3"/>
         <v>9.0242516954262104</v>
       </c>
@@ -10671,26 +10650,26 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <f>('moz2-darwin10-data'!$A$22-'dual-i5-hd-j4'!$B$4) / 60</f>
         <v>92.945894308943082</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>899</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" ref="D5:E5" si="5">C5/$B5</f>
+      <c r="D5" s="8">
+        <f t="shared" ref="D5" si="5">C5/$B5</f>
         <v>9.6722938294811787</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <f t="shared" si="1"/>
         <v>9.1886791380071191</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <f t="shared" si="2"/>
         <v>8.7050644465330613</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <f t="shared" si="3"/>
         <v>7.2542203721108844</v>
       </c>
@@ -10718,26 +10697,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -10800,15 +10779,15 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -13733,26 +13712,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
@@ -13815,15 +13794,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -14049,26 +14028,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -14101,15 +14080,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -14574,26 +14553,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -14626,15 +14605,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -14952,26 +14931,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -15004,15 +14983,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -16894,26 +16873,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -16946,15 +16925,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -17180,26 +17159,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -17232,15 +17211,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -17653,15 +17632,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -17717,15 +17696,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -17808,7 +17787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -17822,113 +17801,113 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="11">
+        <v>35</v>
+      </c>
+      <c r="B3" s="9">
         <f>'quad-i7-ssd-j12'!$B$3</f>
         <v>2371.1999999999998</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <f>24*3600</f>
         <v>86400</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>345</v>
       </c>
       <c r="E3">
         <f>(B3*D3)/C3</f>
         <v>9.4683333333333319</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>1599</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <f>F3*E3</f>
         <v>15139.864999999998</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="11">
+        <v>47</v>
+      </c>
+      <c r="B4" s="9">
         <f>'dual-i7-ssd-j4'!$B$4</f>
         <v>2800.7777777777778</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <f t="shared" ref="C4:C7" si="0">24*3600</f>
         <v>86400</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>345</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E7" si="1">(B4*D4)/C4</f>
         <v>11.183661265432098</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>1699</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="8">
         <f t="shared" ref="G4:G7" si="2">F4*E4</f>
         <v>19001.040489969135</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="11">
+        <v>48</v>
+      </c>
+      <c r="B5" s="9">
         <f>'dual-i7-hd-j4'!$B$4</f>
         <v>2926.6827586206896</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <f t="shared" si="0"/>
         <v>86400</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>345</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
         <v>11.686406848659002</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>1249</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <f t="shared" si="2"/>
         <v>14596.322153975094</v>
       </c>
@@ -17937,25 +17916,25 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <f>'dual-i5-hd-j4'!$B$4</f>
         <v>3578.1463414634145</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>86400</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>345</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
         <v>14.287737127371274</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>899</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <f t="shared" si="2"/>
         <v>12844.675677506775</v>
       </c>
@@ -17968,28 +17947,28 @@
         <f>'moz2-darwin10-data'!$A$22</f>
         <v>9154.9</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>86400</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>345</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
         <v>36.556024305555553</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>0</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -18017,15 +17996,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -18256,26 +18235,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -18338,15 +18317,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -22299,26 +22278,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -22351,15 +22330,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">

</xml_diff>